<commit_message>
Update latest version 2
Latest Version 2 on AMASS Website as of 1 May 2023
</commit_message>
<xml_diff>
--- a/Configuration/Configuration.xlsx
+++ b/Configuration/Configuration.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20383"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20390"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chalida\Downloads\AMASS2\AMASS2.0\Configuration\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chalida\Documents\AMASSv2.0.15_testRun_20221006\AMASSv2.0\Configuration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A675E49-1383-4E7C-8DA0-2130D6019A13}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5ECD106-5D54-436D-B371-B291473323AB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17730" xr2:uid="{3DDA365C-AA97-4E2E-9697-A1BDF02700BD}"/>
   </bookViews>
@@ -171,9 +171,6 @@
     </r>
   </si>
   <si>
-    <t>Generating DATAQC report</t>
-  </si>
-  <si>
     <t>Generating AMR report</t>
   </si>
   <si>
@@ -252,7 +249,10 @@
     </r>
   </si>
   <si>
-    <t>Requirement</t>
+    <t>Requirements</t>
+  </si>
+  <si>
+    <t>Generating Supplementary report</t>
   </si>
 </sst>
 </file>
@@ -666,12 +666,12 @@
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="105" zoomScaleNormal="117" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23.90625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.54296875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.7265625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="83.1796875" bestFit="1" customWidth="1"/>
@@ -685,7 +685,7 @@
         <v>4</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>1</v>
@@ -707,7 +707,7 @@
     </row>
     <row r="3" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>0</v>
@@ -721,7 +721,7 @@
     </row>
     <row r="4" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>0</v>
@@ -730,18 +730,18 @@
         <v>2</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>1</v>
@@ -749,7 +749,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>0</v>
@@ -763,7 +763,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>0</v>
@@ -777,7 +777,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>0</v>
@@ -791,7 +791,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>0</v>
@@ -805,7 +805,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>0</v>
@@ -819,7 +819,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>0</v>
@@ -833,7 +833,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>0</v>
@@ -847,7 +847,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>0</v>
@@ -861,13 +861,13 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>1</v>
@@ -875,7 +875,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>0</v>

</xml_diff>